<commit_message>
making pictures smaller for faster loading
</commit_message>
<xml_diff>
--- a/assets/docs/chinese_vocab_lists.xlsx
+++ b/assets/docs/chinese_vocab_lists.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Electrical" sheetId="1" r:id="rId1"/>
+    <sheet name="Mechanical" sheetId="2" r:id="rId2"/>
+    <sheet name="Wiring" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="249">
   <si>
     <t>电压</t>
   </si>
@@ -318,13 +321,466 @@
   </si>
   <si>
     <t>diànyā</t>
+  </si>
+  <si>
+    <t>Electronics Testing</t>
+  </si>
+  <si>
+    <t>Connector (Male)</t>
+  </si>
+  <si>
+    <t>Connector (Female)</t>
+  </si>
+  <si>
+    <t>Pin (Male)</t>
+  </si>
+  <si>
+    <t>Pin (Female)</t>
+  </si>
+  <si>
+    <t>Supplying Power</t>
+  </si>
+  <si>
+    <t>Constant Current Mode</t>
+  </si>
+  <si>
+    <t>Constant Voltage Mode</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>Grounding</t>
+  </si>
+  <si>
+    <t>接地</t>
+  </si>
+  <si>
+    <t>Insulation (on a wire)</t>
+  </si>
+  <si>
+    <t>导电</t>
+  </si>
+  <si>
+    <t>导电的</t>
+  </si>
+  <si>
+    <t>Conductive</t>
+  </si>
+  <si>
+    <t>To Conduct</t>
+  </si>
+  <si>
+    <t>Insulate</t>
+  </si>
+  <si>
+    <t>Insulation</t>
+  </si>
+  <si>
+    <t>供电</t>
+  </si>
+  <si>
+    <t>保险丝</t>
+  </si>
+  <si>
+    <t>Thermocouple</t>
+  </si>
+  <si>
+    <t>热电偶</t>
+  </si>
+  <si>
+    <t>Aluminum Fixture</t>
+  </si>
+  <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Fasteners</t>
+  </si>
+  <si>
+    <t>摆放</t>
+  </si>
+  <si>
+    <t>Bolt</t>
+  </si>
+  <si>
+    <t>Nut</t>
+  </si>
+  <si>
+    <t>Nylon Locking Nut</t>
+  </si>
+  <si>
+    <t>Ion Chomatography</t>
+  </si>
+  <si>
+    <t>Thermal Chamber</t>
+  </si>
+  <si>
+    <t>HTHE</t>
+  </si>
+  <si>
+    <t>PTCE</t>
+  </si>
+  <si>
+    <t>Salt Fog</t>
+  </si>
+  <si>
+    <t>插头</t>
+  </si>
+  <si>
+    <t>接头</t>
+  </si>
+  <si>
+    <t>绝缘皮层</t>
+  </si>
+  <si>
+    <t>铜芯导线</t>
+  </si>
+  <si>
+    <t>Copper Core Wire</t>
+  </si>
+  <si>
+    <t>绝缘电阻测试</t>
+  </si>
+  <si>
+    <t>Insulation Resistance Test</t>
+  </si>
+  <si>
+    <t>Hipot Test</t>
+  </si>
+  <si>
+    <t>Wiring Harness</t>
+  </si>
+  <si>
+    <t>线束、线</t>
+  </si>
+  <si>
+    <t>公头</t>
+  </si>
+  <si>
+    <t>Male Connector</t>
+  </si>
+  <si>
+    <t>Female Connector</t>
+  </si>
+  <si>
+    <t>BNC Connector</t>
+  </si>
+  <si>
+    <t>公母头</t>
+  </si>
+  <si>
+    <t xml:space="preserve">母头 </t>
+  </si>
+  <si>
+    <t>插座</t>
+  </si>
+  <si>
+    <t>Receptacle/Outlet</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>印刷电路板、板子</t>
+  </si>
+  <si>
+    <t>Buzzer (piezo)</t>
+  </si>
+  <si>
+    <t>蜂鸣器</t>
+  </si>
+  <si>
+    <t>用途</t>
+  </si>
+  <si>
+    <t>use/application</t>
+  </si>
+  <si>
+    <t>传递电信号</t>
+  </si>
+  <si>
+    <t>Signal Transmission</t>
+  </si>
+  <si>
+    <t>信号处理</t>
+  </si>
+  <si>
+    <t>Signal Processing</t>
+  </si>
+  <si>
+    <t>DSP Chip</t>
+  </si>
+  <si>
+    <t>数字信号处理芯片、DSP芯片</t>
+  </si>
+  <si>
+    <t>Screens</t>
+  </si>
+  <si>
+    <t>盐雾实验</t>
+  </si>
+  <si>
+    <t>高温高湿实验</t>
+  </si>
+  <si>
+    <t>快速变温实验</t>
+  </si>
+  <si>
+    <t>压接工具</t>
+  </si>
+  <si>
+    <t>Crimp Tool</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>Drill</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Ratchet</t>
+  </si>
+  <si>
+    <t>Socket Wrench</t>
+  </si>
+  <si>
+    <t>Socket Heads</t>
+  </si>
+  <si>
+    <t>Screw Driver</t>
+  </si>
+  <si>
+    <t>Diagonal/Flush Cutters</t>
+  </si>
+  <si>
+    <t>Needle Nose Pliers</t>
+  </si>
+  <si>
+    <t>Electrical Tape</t>
+  </si>
+  <si>
+    <t>绝缘带</t>
+  </si>
+  <si>
+    <t>Ethernet Cable</t>
+  </si>
+  <si>
+    <t>网线</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>路由器</t>
+  </si>
+  <si>
+    <t>猫</t>
+  </si>
+  <si>
+    <t>Modem</t>
+  </si>
+  <si>
+    <t>Sold而ing Iron</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Water Soluble Flux</t>
+  </si>
+  <si>
+    <t>No-clean Flux</t>
+  </si>
+  <si>
+    <t>Solder Paste</t>
+  </si>
+  <si>
+    <t>Solder Wick</t>
+  </si>
+  <si>
+    <t>Semiconductor</t>
+  </si>
+  <si>
+    <t>半导体</t>
+  </si>
+  <si>
+    <t>Discrete Components</t>
+  </si>
+  <si>
+    <t>分立元件</t>
+  </si>
+  <si>
+    <t>热管理</t>
+  </si>
+  <si>
+    <t>Thermal Management</t>
+  </si>
+  <si>
+    <t>电阻器</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>线圈</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>扼流圈</t>
+  </si>
+  <si>
+    <t>Choke</t>
+  </si>
+  <si>
+    <t>Thermal Test Chamber</t>
+  </si>
+  <si>
+    <t>试验箱</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>电位计</t>
+  </si>
+  <si>
+    <t>晶体</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Oscillator</t>
+  </si>
+  <si>
+    <t>振荡器</t>
+  </si>
+  <si>
+    <t>光电</t>
+  </si>
+  <si>
+    <t>Photoelectric</t>
+  </si>
+  <si>
+    <t>嵌入式电脑</t>
+  </si>
+  <si>
+    <t>Embedded Computer / Embedded Computing</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>射频</t>
+  </si>
+  <si>
+    <t>Radio Frequency (RF)</t>
+  </si>
+  <si>
+    <t>传感器</t>
+  </si>
+  <si>
+    <t>Sensor/Transducer</t>
+  </si>
+  <si>
+    <t>变送器</t>
+  </si>
+  <si>
+    <t>Transmitter</t>
+  </si>
+  <si>
+    <t>滤波器</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>变压器</t>
+  </si>
+  <si>
+    <t>Transformer</t>
+  </si>
+  <si>
+    <t>TVS二极管</t>
+  </si>
+  <si>
+    <t>TVS Diode</t>
+  </si>
+  <si>
+    <t>阵列</t>
+  </si>
+  <si>
+    <t>Switching (diode, mosfet)</t>
+  </si>
+  <si>
+    <t>FET</t>
+  </si>
+  <si>
+    <t>硅晶体管</t>
+  </si>
+  <si>
+    <t>Silicon Transistor</t>
+  </si>
+  <si>
+    <t>双极晶体管</t>
+  </si>
+  <si>
+    <t>DMM</t>
+  </si>
+  <si>
+    <t>万用表</t>
+  </si>
+  <si>
+    <t>焊</t>
+  </si>
+  <si>
+    <t>助焊剂</t>
+  </si>
+  <si>
+    <t>电源</t>
+  </si>
+  <si>
+    <t>示波器</t>
+  </si>
+  <si>
+    <t>探针、</t>
+  </si>
+  <si>
+    <t>Quiescent Current</t>
+  </si>
+  <si>
+    <t>Electric Motor</t>
+  </si>
+  <si>
+    <t>电机</t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>DC Brushed Motor</t>
+  </si>
+  <si>
+    <t>BLDC</t>
+  </si>
+  <si>
+    <t>Permanent Magnet Motor</t>
+  </si>
+  <si>
+    <t>Induction Motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +806,26 @@
       <color rgb="FF252525"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -384,10 +860,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -407,8 +884,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H57"/>
+  <dimension ref="B1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -698,14 +1191,21 @@
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:14">
       <c r="B1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -715,8 +1215,23 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -726,8 +1241,21 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="G4" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -737,8 +1265,21 @@
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="G5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" t="s">
+        <v>146</v>
+      </c>
+      <c r="N5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -748,8 +1289,21 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="G6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -759,8 +1313,19 @@
       <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="G7" s="4"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" t="s">
+        <v>151</v>
+      </c>
+      <c r="N7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -770,8 +1335,19 @@
       <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="G8" s="4"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -781,8 +1357,21 @@
       <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="G9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" t="s">
+        <v>154</v>
+      </c>
+      <c r="N9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -792,8 +1381,21 @@
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
+      <c r="G10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -803,53 +1405,119 @@
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="2:4">
+      <c r="G11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M11" t="s">
+        <v>158</v>
+      </c>
+      <c r="N11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
+      <c r="G12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="N12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="2:4">
+      <c r="D13" s="7"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" t="s">
+        <v>166</v>
+      </c>
+      <c r="N13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="2:4">
+      <c r="G14" s="4"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="D15" s="7"/>
+      <c r="G15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="G17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="I18" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -859,8 +1527,14 @@
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="2:4">
+      <c r="G19" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
@@ -870,8 +1544,11 @@
       <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
@@ -881,8 +1558,14 @@
       <c r="D21" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="N21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
@@ -892,8 +1575,17 @@
       <c r="D22" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
+      <c r="G22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" t="s">
+        <v>106</v>
+      </c>
+      <c r="N22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" s="3" t="s">
         <v>39</v>
       </c>
@@ -903,8 +1595,17 @@
       <c r="D23" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="2:4">
+      <c r="G23" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" t="s">
+        <v>118</v>
+      </c>
+      <c r="N23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" s="3" t="s">
         <v>50</v>
       </c>
@@ -914,8 +1615,14 @@
       <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="2:4">
+      <c r="I24" t="s">
+        <v>120</v>
+      </c>
+      <c r="N24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
@@ -925,28 +1632,49 @@
       <c r="D25" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="2:4">
+      <c r="G25" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" t="s">
+        <v>121</v>
+      </c>
+      <c r="N25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="2:4">
+      <c r="I26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="B27" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="2:4">
+      <c r="D27" s="7"/>
+      <c r="I27" t="s">
+        <v>124</v>
+      </c>
+      <c r="N27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
@@ -956,8 +1684,14 @@
       <c r="D28" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="2:4">
+      <c r="I28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29" s="3" t="s">
         <v>53</v>
       </c>
@@ -967,8 +1701,17 @@
       <c r="D29" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="2:4">
+      <c r="I29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M29" t="s">
+        <v>178</v>
+      </c>
+      <c r="N29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="B30" s="3" t="s">
         <v>52</v>
       </c>
@@ -979,7 +1722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:14">
       <c r="B31" s="3" t="s">
         <v>38</v>
       </c>
@@ -989,24 +1732,50 @@
       <c r="D31" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="2:8">
+      <c r="I31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="I32" t="s">
+        <v>128</v>
+      </c>
+      <c r="M32" t="s">
+        <v>180</v>
+      </c>
+      <c r="N32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
       <c r="D33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="H33" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="2:8">
+      <c r="M33" t="s">
+        <v>182</v>
+      </c>
+      <c r="N33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
       <c r="D34" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H34" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="2:8">
+      <c r="M34" t="s">
+        <v>183</v>
+      </c>
+      <c r="N34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -1014,46 +1783,88 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:14">
       <c r="B36" t="s">
         <v>76</v>
       </c>
       <c r="D36" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="2:8">
+      <c r="G36" t="s">
+        <v>164</v>
+      </c>
+      <c r="I36" t="s">
+        <v>129</v>
+      </c>
+      <c r="N36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
       <c r="B37" t="s">
         <v>69</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="2:8">
+      <c r="G37" t="s">
+        <v>165</v>
+      </c>
+      <c r="I37" t="s">
+        <v>130</v>
+      </c>
+      <c r="N37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
       <c r="B38" t="s">
         <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="2:8">
+      <c r="G38" t="s">
+        <v>163</v>
+      </c>
+      <c r="I38" t="s">
+        <v>131</v>
+      </c>
+      <c r="N38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
       <c r="D39" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="2:8">
+      <c r="N39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
       <c r="D40" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="2:8">
+      <c r="N40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
       <c r="D41" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="2:8">
+      <c r="G41" t="s">
+        <v>204</v>
+      </c>
+      <c r="I41" t="s">
+        <v>203</v>
+      </c>
+      <c r="N41" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
       <c r="B42" t="s">
         <v>75</v>
       </c>
@@ -1061,65 +1872,256 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:14">
       <c r="D43" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="2:8">
+      <c r="M43" t="s">
+        <v>192</v>
+      </c>
+      <c r="N43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
       <c r="B44" t="s">
         <v>72</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="45" spans="2:8">
+      <c r="M44" t="s">
+        <v>194</v>
+      </c>
+      <c r="N44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
       <c r="B45" t="s">
         <v>74</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="4:4">
+      <c r="M45" t="s">
+        <v>195</v>
+      </c>
+      <c r="N45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="M46" t="s">
+        <v>197</v>
+      </c>
+      <c r="N46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="M47" t="s">
+        <v>199</v>
+      </c>
+      <c r="N47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="M48" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14">
+      <c r="M49" t="s">
+        <v>201</v>
+      </c>
+      <c r="N49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14">
+      <c r="C50" t="s">
+        <v>238</v>
+      </c>
       <c r="D50" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="4:4">
+      <c r="M50" t="s">
+        <v>206</v>
+      </c>
+      <c r="N50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14">
+      <c r="C51" t="s">
+        <v>239</v>
+      </c>
       <c r="D51" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="4:4">
+      <c r="M51" t="s">
+        <v>207</v>
+      </c>
+      <c r="N51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14">
+      <c r="C52" t="s">
+        <v>240</v>
+      </c>
       <c r="D52" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="53" spans="4:4">
+      <c r="M52" t="s">
+        <v>210</v>
+      </c>
+      <c r="N52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14">
       <c r="D53" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="54" spans="4:4">
+      <c r="M53" t="s">
+        <v>211</v>
+      </c>
+      <c r="N53" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14">
       <c r="D54" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="4:4">
+      <c r="M54" t="s">
+        <v>213</v>
+      </c>
+      <c r="N54" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="3:14">
       <c r="D55" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="56" spans="4:4">
+      <c r="M55" t="s">
+        <v>51</v>
+      </c>
+      <c r="N55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14">
+      <c r="C56" t="s">
+        <v>236</v>
+      </c>
       <c r="D56" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="57" spans="4:4">
+      <c r="M56" t="s">
+        <v>216</v>
+      </c>
+      <c r="N56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="3:14">
+      <c r="C57" t="s">
+        <v>237</v>
+      </c>
       <c r="D57" t="s">
         <v>85</v>
+      </c>
+      <c r="M57" t="s">
+        <v>218</v>
+      </c>
+      <c r="N57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14">
+      <c r="C58" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" t="s">
+        <v>234</v>
+      </c>
+      <c r="M58" t="s">
+        <v>220</v>
+      </c>
+      <c r="N58" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="3:14">
+      <c r="M59" t="s">
+        <v>222</v>
+      </c>
+      <c r="N59" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14">
+      <c r="M60" t="s">
+        <v>224</v>
+      </c>
+      <c r="N60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="3:14">
+      <c r="M61" t="s">
+        <v>226</v>
+      </c>
+      <c r="N61" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="3:14">
+      <c r="M62" t="s">
+        <v>228</v>
+      </c>
+      <c r="N62" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="3:14">
+      <c r="M63" t="s">
+        <v>50</v>
+      </c>
+      <c r="N63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="3:14">
+      <c r="M64" t="s">
+        <v>230</v>
+      </c>
+      <c r="N64" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="13:14">
+      <c r="M65" t="s">
+        <v>233</v>
+      </c>
+      <c r="N65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="13:14">
+      <c r="M66" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="N66" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +2130,90 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D26:D27"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M66" r:id="rId1" tooltip="查看 硅晶体管" display="https://image.baidu.com/search/index?ct=201326592&amp;cl=2&amp;st=-1&amp;lm=-1&amp;nc=1&amp;ie=utf-8&amp;tn=baiduimage&amp;ipn=r&amp;rps=1&amp;pv=&amp;fm=rs4&amp;word=%E7%A1%85%E6%99%B6%E4%BD%93%E7%AE%A1&amp;oriquery=%E6%99%B6%E4%BD%93%E7%AE%A1%E4%BA%8C%E7%BA%A7&amp;ofr=%E6%99%B6%E4%BD%93%E7%AE%A1%E4%BA%8C%E7%BA%A7&amp;ctd=1489674287717%5e00_1903X950"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>